<commit_message>
backend did lots change
</commit_message>
<xml_diff>
--- a/backend/Building.xlsx
+++ b/backend/Building.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlos/MyCampus/backend/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\Desktop\新建文件夹\MyCampus\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CA598D7-B1EB-F145-BA95-BA0B1466D96E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4E8F133-7465-438D-A853-A13DCFEFB0C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="20700" windowHeight="12080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="162">
   <si>
     <t>Central Podium Levels</t>
   </si>
@@ -518,6 +518,12 @@
   <si>
     <t>Coordinate</t>
     <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>WCL</t>
+  </si>
+  <si>
+    <t>WCM</t>
   </si>
 </sst>
 </file>
@@ -528,7 +534,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -553,7 +559,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -895,19 +901,19 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="32.83203125" customWidth="1"/>
-    <col min="2" max="2" width="29.83203125" customWidth="1"/>
-    <col min="3" max="3" width="45.83203125" customWidth="1"/>
+    <col min="1" max="1" width="32.85546875" customWidth="1"/>
+    <col min="2" max="2" width="29.85546875" customWidth="1"/>
+    <col min="3" max="3" width="45.85546875" customWidth="1"/>
     <col min="4" max="4" width="59" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17">
+    <row r="1" spans="1:5" ht="16.5">
       <c r="A1" s="1" t="s">
         <v>155</v>
       </c>
@@ -1109,7 +1115,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" ht="25.5">
       <c r="A13" s="1" t="s">
         <v>53</v>
       </c>
@@ -1211,7 +1217,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" ht="25.5">
       <c r="A19" s="5" t="s">
         <v>80</v>
       </c>
@@ -1245,7 +1251,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15">
+    <row r="21" spans="1:5">
       <c r="A21" s="5" t="s">
         <v>88</v>
       </c>
@@ -1479,7 +1485,9 @@
       <c r="D34" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E34" s="1"/>
+      <c r="E34" s="1" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="5" t="s">
@@ -1494,7 +1502,9 @@
       <c r="D35" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E35" s="1"/>
+      <c r="E35" s="1" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="5" t="s">

</xml_diff>

<commit_message>
Checkpoint 1 & 2 backend finished
</commit_message>
<xml_diff>
--- a/backend/Building.xlsx
+++ b/backend/Building.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\Desktop\新建文件夹\MyCampus\backend\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\Desktop\p\MyCampus\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4E8F133-7465-438D-A853-A13DCFEFB0C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F473176D-7547-421B-9415-80D646097ED6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17340" yWindow="0" windowWidth="11565" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="159">
   <si>
     <t>Central Podium Levels</t>
   </si>
@@ -453,18 +453,6 @@
   </si>
   <si>
     <t>TC</t>
-  </si>
-  <si>
-    <t>The Jockey Club Tower</t>
-  </si>
-  <si>
-    <t>賽馬會教學樓</t>
-  </si>
-  <si>
-    <t>22.28184475858962, 114.13744558806208</t>
-  </si>
-  <si>
-    <t>CJT</t>
   </si>
   <si>
     <t>Wong Chuang Lai Wah Building</t>
@@ -524,6 +512,9 @@
   </si>
   <si>
     <t>WCM</t>
+  </si>
+  <si>
+    <t>CYCC</t>
   </si>
 </sst>
 </file>
@@ -898,10 +889,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -915,19 +906,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="16.5">
       <c r="A1" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>159</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1011,7 +1002,9 @@
       <c r="D6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="1"/>
+      <c r="E6" s="1" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="4" t="s">
@@ -1469,58 +1462,41 @@
         <v>41</v>
       </c>
       <c r="E33" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="5" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="1" t="s">
+      <c r="B34" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>146</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>41</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B35" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="C35" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="D35" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="D35" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="5" t="s">
+      <c r="E35" s="5" t="s">
         <v>150</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>